<commit_message>
handle miss align pop up browser and multi selection
</commit_message>
<xml_diff>
--- a/final/temp.xlsx
+++ b/final/temp.xlsx
@@ -586,12 +586,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>D:\output_beca\549_BeCa_Ghep.mp4</t>
+          <t>D:\video tmp\152 Bé cá.mp4</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -660,12 +660,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>D:\output_beca\550_BeCa_Ghep.mp4</t>
+          <t>D:\video tmp\153 Bé cá.mp4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -734,12 +734,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>D:\output_beca\550_BeCa_Ghep.mp4</t>
+          <t>D:\video tmp\152 Bé cá.mp4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">

</xml_diff>